<commit_message>
casos de prueba de plan y encuesta
</commit_message>
<xml_diff>
--- a/Docs/08-Prueba/TC- Planificacion .xlsx
+++ b/Docs/08-Prueba/TC- Planificacion .xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="147">
   <si>
     <t>Application</t>
   </si>
@@ -523,6 +523,18 @@
   </si>
   <si>
     <t>no permite emilinar contenido que ya estan asociados en registros de clase o en planificacion anual.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Defect </t>
+  </si>
+  <si>
+    <t>defect</t>
+  </si>
+  <si>
+    <t>defcet</t>
+  </si>
+  <si>
+    <t>pass</t>
   </si>
 </sst>
 </file>
@@ -608,7 +620,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -666,6 +678,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -790,7 +808,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -902,70 +920,19 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -977,6 +944,102 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1283,468 +1346,468 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="127.85546875" style="51" customWidth="1"/>
+    <col min="2" max="2" width="127.85546875" style="40" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" customWidth="1"/>
     <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="C1" s="63" t="s">
+      <c r="C1" s="46" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="90">
-      <c r="A2" s="64" t="str">
+      <c r="A2" s="47" t="str">
         <f>US_1!B4</f>
         <v>TC1_US1</v>
       </c>
-      <c r="B2" s="64" t="str">
+      <c r="B2" s="47" t="str">
         <f>US_1!C4</f>
         <v xml:space="preserve"> Objetivo:probar que registrar un contenidos con todos los datos completos y correstos. Asociar contenidos oficiales.
 Pre-condición: Loguearse como Usuario de perfil Docente(user:macosta)
 post-condición:  ---</v>
       </c>
-      <c r="C2" s="64" t="str">
+      <c r="C2" s="47" t="str">
         <f>US_1!G4</f>
         <v>paso</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="75">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="63" t="str">
+      <c r="B3" s="46" t="str">
         <f>US_1!C13</f>
         <v xml:space="preserve">Objetivo: Probar que no debe registrar planificacion con rango de fecha superior al ciclo lectivo Actual.
 Pre-condicion:
 Post-Condicion: no registrar pln fuera del periodo del ciclo lectivo actual. </v>
       </c>
-      <c r="C3" s="63"/>
+      <c r="C3" s="46"/>
     </row>
     <row r="4" spans="1:3" ht="75">
-      <c r="A4" s="63" t="s">
+      <c r="A4" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="63" t="str">
+      <c r="B4" s="46" t="str">
         <f>US_1!C20</f>
         <v xml:space="preserve">Objetivo: Registrar un nuevo contenido de planificacin, cuando ya esta aprobada la planificacion.
 Pre-condicion: la planificacion anual ya fue creada y aprobada por el directos. 
 Post-Condicion:No permite editar contenidos, no se realiza ninguna modificacion en el plan ya aprobado. </v>
       </c>
-      <c r="C4" s="63"/>
+      <c r="C4" s="46"/>
     </row>
     <row r="5" spans="1:3" ht="75">
-      <c r="A5" s="63" t="s">
+      <c r="A5" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="63" t="str">
+      <c r="B5" s="46" t="str">
         <f>US_1!C25</f>
         <v>Objetivo:planificar el mismo contenido varias en distintos periodos.
 Pre-condicion:
 Post-Condicion:</v>
       </c>
-      <c r="C5" s="63"/>
+      <c r="C5" s="46"/>
     </row>
     <row r="6" spans="1:3" ht="90">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="B6" s="63" t="str">
+      <c r="B6" s="46" t="str">
         <f>US_1!C31</f>
         <v>Objetivo:solapamiento fechas de planificacion.
 Pre-condicion:registro de planificacion en la fecha de 02/05/2012
 docente : mdeleonardis
 Post-Condicion:</v>
       </c>
-      <c r="C6" s="63"/>
+      <c r="C6" s="46"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="63" t="s">
+      <c r="A7" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="B7" s="63"/>
-      <c r="C7" s="63"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="63" t="s">
+      <c r="A8" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="B8" s="63"/>
-      <c r="C8" s="63"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="63"/>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
+      <c r="A9" s="46"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="63"/>
-      <c r="B10" s="63"/>
-      <c r="C10" s="63"/>
+      <c r="A10" s="46"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="46"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="63"/>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
+      <c r="A11" s="46"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="46"/>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="63"/>
-      <c r="B12" s="63"/>
-      <c r="C12" s="63"/>
+      <c r="A12" s="46"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="46"/>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="63"/>
-      <c r="B13" s="63"/>
-      <c r="C13" s="63"/>
+      <c r="A13" s="46"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="46"/>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="63"/>
-      <c r="B14" s="63"/>
-      <c r="C14" s="63"/>
+      <c r="A14" s="46"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="46"/>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="63"/>
-      <c r="B15" s="63"/>
-      <c r="C15" s="63"/>
+      <c r="A15" s="46"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="46"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="63"/>
-      <c r="B16" s="63"/>
-      <c r="C16" s="63"/>
+      <c r="A16" s="46"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="46"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="63"/>
-      <c r="B17" s="63"/>
-      <c r="C17" s="63"/>
+      <c r="A17" s="46"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="46"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="63"/>
-      <c r="B18" s="63"/>
-      <c r="C18" s="63"/>
+      <c r="A18" s="46"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="46"/>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="63"/>
-      <c r="B19" s="63"/>
-      <c r="C19" s="63"/>
+      <c r="A19" s="46"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="46"/>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="63"/>
-      <c r="B20" s="63"/>
-      <c r="C20" s="63"/>
+      <c r="A20" s="46"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="46"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="63"/>
-      <c r="B21" s="63"/>
-      <c r="C21" s="63"/>
+      <c r="A21" s="46"/>
+      <c r="B21" s="46"/>
+      <c r="C21" s="46"/>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="63"/>
-      <c r="B22" s="63"/>
-      <c r="C22" s="63"/>
+      <c r="A22" s="46"/>
+      <c r="B22" s="46"/>
+      <c r="C22" s="46"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="63"/>
-      <c r="B23" s="63"/>
-      <c r="C23" s="63"/>
+      <c r="A23" s="46"/>
+      <c r="B23" s="46"/>
+      <c r="C23" s="46"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="63"/>
-      <c r="B24" s="63"/>
-      <c r="C24" s="63"/>
+      <c r="A24" s="46"/>
+      <c r="B24" s="46"/>
+      <c r="C24" s="46"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="63"/>
-      <c r="B25" s="63"/>
-      <c r="C25" s="63"/>
+      <c r="A25" s="46"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="46"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="63"/>
-      <c r="B26" s="63"/>
-      <c r="C26" s="63"/>
+      <c r="A26" s="46"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="46"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="63"/>
-      <c r="B27" s="63"/>
-      <c r="C27" s="63"/>
+      <c r="A27" s="46"/>
+      <c r="B27" s="46"/>
+      <c r="C27" s="46"/>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="63"/>
-      <c r="B28" s="63"/>
-      <c r="C28" s="63"/>
+      <c r="A28" s="46"/>
+      <c r="B28" s="46"/>
+      <c r="C28" s="46"/>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="63"/>
-      <c r="B29" s="63"/>
-      <c r="C29" s="63"/>
+      <c r="A29" s="46"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="63"/>
-      <c r="B30" s="63"/>
-      <c r="C30" s="63"/>
+      <c r="A30" s="46"/>
+      <c r="B30" s="46"/>
+      <c r="C30" s="46"/>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="63"/>
-      <c r="B31" s="63"/>
-      <c r="C31" s="63"/>
+      <c r="A31" s="46"/>
+      <c r="B31" s="46"/>
+      <c r="C31" s="46"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="63"/>
-      <c r="B32" s="63"/>
-      <c r="C32" s="63"/>
+      <c r="A32" s="46"/>
+      <c r="B32" s="46"/>
+      <c r="C32" s="46"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="63"/>
-      <c r="B33" s="63"/>
-      <c r="C33" s="63"/>
+      <c r="A33" s="46"/>
+      <c r="B33" s="46"/>
+      <c r="C33" s="46"/>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="63"/>
-      <c r="B34" s="63"/>
-      <c r="C34" s="63"/>
+      <c r="A34" s="46"/>
+      <c r="B34" s="46"/>
+      <c r="C34" s="46"/>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="63"/>
-      <c r="B35" s="63"/>
-      <c r="C35" s="63"/>
+      <c r="A35" s="46"/>
+      <c r="B35" s="46"/>
+      <c r="C35" s="46"/>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="63"/>
-      <c r="B36" s="63"/>
-      <c r="C36" s="63"/>
+      <c r="A36" s="46"/>
+      <c r="B36" s="46"/>
+      <c r="C36" s="46"/>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="63"/>
-      <c r="B37" s="63"/>
-      <c r="C37" s="63"/>
+      <c r="A37" s="46"/>
+      <c r="B37" s="46"/>
+      <c r="C37" s="46"/>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="63"/>
-      <c r="B38" s="63"/>
-      <c r="C38" s="63"/>
+      <c r="A38" s="46"/>
+      <c r="B38" s="46"/>
+      <c r="C38" s="46"/>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="63"/>
-      <c r="B39" s="63"/>
-      <c r="C39" s="63"/>
+      <c r="A39" s="46"/>
+      <c r="B39" s="46"/>
+      <c r="C39" s="46"/>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="63"/>
-      <c r="B40" s="63"/>
-      <c r="C40" s="63"/>
+      <c r="A40" s="46"/>
+      <c r="B40" s="46"/>
+      <c r="C40" s="46"/>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="63"/>
-      <c r="B41" s="63"/>
-      <c r="C41" s="63"/>
+      <c r="A41" s="46"/>
+      <c r="B41" s="46"/>
+      <c r="C41" s="46"/>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="63"/>
-      <c r="B42" s="63"/>
-      <c r="C42" s="63"/>
+      <c r="A42" s="46"/>
+      <c r="B42" s="46"/>
+      <c r="C42" s="46"/>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="63"/>
-      <c r="B43" s="63"/>
-      <c r="C43" s="63"/>
+      <c r="A43" s="46"/>
+      <c r="B43" s="46"/>
+      <c r="C43" s="46"/>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="63"/>
-      <c r="B44" s="63"/>
-      <c r="C44" s="63"/>
+      <c r="A44" s="46"/>
+      <c r="B44" s="46"/>
+      <c r="C44" s="46"/>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="63"/>
-      <c r="B45" s="63"/>
-      <c r="C45" s="63"/>
+      <c r="A45" s="46"/>
+      <c r="B45" s="46"/>
+      <c r="C45" s="46"/>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="63"/>
-      <c r="B46" s="63"/>
-      <c r="C46" s="63"/>
+      <c r="A46" s="46"/>
+      <c r="B46" s="46"/>
+      <c r="C46" s="46"/>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="63"/>
-      <c r="B47" s="63"/>
-      <c r="C47" s="63"/>
+      <c r="A47" s="46"/>
+      <c r="B47" s="46"/>
+      <c r="C47" s="46"/>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="63"/>
-      <c r="B48" s="63"/>
-      <c r="C48" s="63"/>
+      <c r="A48" s="46"/>
+      <c r="B48" s="46"/>
+      <c r="C48" s="46"/>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="63"/>
-      <c r="B49" s="63"/>
-      <c r="C49" s="63"/>
+      <c r="A49" s="46"/>
+      <c r="B49" s="46"/>
+      <c r="C49" s="46"/>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="63"/>
-      <c r="B50" s="63"/>
-      <c r="C50" s="63"/>
+      <c r="A50" s="46"/>
+      <c r="B50" s="46"/>
+      <c r="C50" s="46"/>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="63"/>
-      <c r="B51" s="63"/>
-      <c r="C51" s="63"/>
+      <c r="A51" s="46"/>
+      <c r="B51" s="46"/>
+      <c r="C51" s="46"/>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="63"/>
-      <c r="B52" s="63"/>
-      <c r="C52" s="63"/>
+      <c r="A52" s="46"/>
+      <c r="B52" s="46"/>
+      <c r="C52" s="46"/>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="63"/>
-      <c r="B53" s="63"/>
-      <c r="C53" s="63"/>
+      <c r="A53" s="46"/>
+      <c r="B53" s="46"/>
+      <c r="C53" s="46"/>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="63"/>
-      <c r="B54" s="63"/>
-      <c r="C54" s="63"/>
+      <c r="A54" s="46"/>
+      <c r="B54" s="46"/>
+      <c r="C54" s="46"/>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="63"/>
-      <c r="B55" s="63"/>
-      <c r="C55" s="63"/>
+      <c r="A55" s="46"/>
+      <c r="B55" s="46"/>
+      <c r="C55" s="46"/>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" s="63"/>
-      <c r="B56" s="63"/>
-      <c r="C56" s="63"/>
+      <c r="A56" s="46"/>
+      <c r="B56" s="46"/>
+      <c r="C56" s="46"/>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" s="63"/>
-      <c r="B57" s="63"/>
-      <c r="C57" s="63"/>
+      <c r="A57" s="46"/>
+      <c r="B57" s="46"/>
+      <c r="C57" s="46"/>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" s="63"/>
-      <c r="B58" s="63"/>
-      <c r="C58" s="63"/>
+      <c r="A58" s="46"/>
+      <c r="B58" s="46"/>
+      <c r="C58" s="46"/>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" s="63"/>
-      <c r="B59" s="63"/>
-      <c r="C59" s="63"/>
+      <c r="A59" s="46"/>
+      <c r="B59" s="46"/>
+      <c r="C59" s="46"/>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="63"/>
-      <c r="B60" s="63"/>
-      <c r="C60" s="63"/>
+      <c r="A60" s="46"/>
+      <c r="B60" s="46"/>
+      <c r="C60" s="46"/>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="63"/>
-      <c r="B61" s="63"/>
-      <c r="C61" s="63"/>
+      <c r="A61" s="46"/>
+      <c r="B61" s="46"/>
+      <c r="C61" s="46"/>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="63"/>
-      <c r="B62" s="63"/>
-      <c r="C62" s="63"/>
+      <c r="A62" s="46"/>
+      <c r="B62" s="46"/>
+      <c r="C62" s="46"/>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" s="63"/>
-      <c r="B63" s="63"/>
-      <c r="C63" s="63"/>
+      <c r="A63" s="46"/>
+      <c r="B63" s="46"/>
+      <c r="C63" s="46"/>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" s="63"/>
-      <c r="B64" s="63"/>
-      <c r="C64" s="63"/>
+      <c r="A64" s="46"/>
+      <c r="B64" s="46"/>
+      <c r="C64" s="46"/>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" s="63"/>
-      <c r="B65" s="63"/>
-      <c r="C65" s="63"/>
+      <c r="A65" s="46"/>
+      <c r="B65" s="46"/>
+      <c r="C65" s="46"/>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="63"/>
-      <c r="B66" s="63"/>
-      <c r="C66" s="63"/>
+      <c r="A66" s="46"/>
+      <c r="B66" s="46"/>
+      <c r="C66" s="46"/>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" s="63"/>
-      <c r="B67" s="63"/>
-      <c r="C67" s="63"/>
+      <c r="A67" s="46"/>
+      <c r="B67" s="46"/>
+      <c r="C67" s="46"/>
     </row>
     <row r="68" spans="1:3">
-      <c r="A68" s="63"/>
-      <c r="B68" s="63"/>
-      <c r="C68" s="63"/>
+      <c r="A68" s="46"/>
+      <c r="B68" s="46"/>
+      <c r="C68" s="46"/>
     </row>
     <row r="69" spans="1:3">
-      <c r="A69" s="63"/>
-      <c r="B69" s="63"/>
-      <c r="C69" s="63"/>
+      <c r="A69" s="46"/>
+      <c r="B69" s="46"/>
+      <c r="C69" s="46"/>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="63"/>
-      <c r="B70" s="63"/>
-      <c r="C70" s="63"/>
+      <c r="A70" s="46"/>
+      <c r="B70" s="46"/>
+      <c r="C70" s="46"/>
     </row>
     <row r="71" spans="1:3">
-      <c r="A71" s="63"/>
-      <c r="B71" s="63"/>
-      <c r="C71" s="63"/>
+      <c r="A71" s="46"/>
+      <c r="B71" s="46"/>
+      <c r="C71" s="46"/>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" s="63"/>
-      <c r="B72" s="63"/>
-      <c r="C72" s="63"/>
+      <c r="A72" s="46"/>
+      <c r="B72" s="46"/>
+      <c r="C72" s="46"/>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="63"/>
-      <c r="B73" s="63"/>
-      <c r="C73" s="63"/>
+      <c r="A73" s="46"/>
+      <c r="B73" s="46"/>
+      <c r="C73" s="46"/>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="63"/>
-      <c r="B74" s="63"/>
-      <c r="C74" s="63"/>
+      <c r="A74" s="46"/>
+      <c r="B74" s="46"/>
+      <c r="C74" s="46"/>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="63"/>
-      <c r="B75" s="63"/>
-      <c r="C75" s="63"/>
+      <c r="A75" s="46"/>
+      <c r="B75" s="46"/>
+      <c r="C75" s="46"/>
     </row>
     <row r="76" spans="1:3">
-      <c r="A76" s="63"/>
-      <c r="B76" s="63"/>
-      <c r="C76" s="63"/>
+      <c r="A76" s="46"/>
+      <c r="B76" s="46"/>
+      <c r="C76" s="46"/>
     </row>
     <row r="77" spans="1:3">
-      <c r="A77" s="63"/>
-      <c r="B77" s="63"/>
-      <c r="C77" s="63"/>
+      <c r="A77" s="46"/>
+      <c r="B77" s="46"/>
+      <c r="C77" s="46"/>
     </row>
     <row r="78" spans="1:3">
-      <c r="A78" s="63"/>
-      <c r="B78" s="63"/>
-      <c r="C78" s="63"/>
+      <c r="A78" s="46"/>
+      <c r="B78" s="46"/>
+      <c r="C78" s="46"/>
     </row>
     <row r="79" spans="1:3">
-      <c r="A79" s="63"/>
-      <c r="B79" s="63"/>
-      <c r="C79" s="63"/>
+      <c r="A79" s="46"/>
+      <c r="B79" s="46"/>
+      <c r="C79" s="46"/>
     </row>
     <row r="80" spans="1:3">
-      <c r="A80" s="63"/>
-      <c r="B80" s="63"/>
-      <c r="C80" s="63"/>
+      <c r="A80" s="46"/>
+      <c r="B80" s="46"/>
+      <c r="C80" s="46"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1753,10 +1816,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1766,19 +1829,20 @@
     <col min="6" max="6" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="40.5" customHeight="1" thickBot="1">
-      <c r="A1" s="50" t="s">
+    <row r="1" spans="1:9" ht="40.5" customHeight="1" thickBot="1">
+      <c r="A1" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1">
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1801,10 +1865,13 @@
         <v>6</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1826,63 +1893,68 @@
       <c r="G3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="4"/>
+      <c r="I3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A4" s="37" t="s">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A4" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="42"/>
+      <c r="C4" s="68"/>
       <c r="D4" s="5">
         <v>1</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="6"/>
-      <c r="G4" s="37"/>
+      <c r="G4" s="54"/>
       <c r="H4" s="37"/>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A5" s="38"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="43"/>
+      <c r="I4" s="54"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A5" s="55"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="69"/>
       <c r="D5" s="5">
         <v>2</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="6"/>
-      <c r="G5" s="38"/>
+      <c r="G5" s="55"/>
       <c r="H5" s="38"/>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A6" s="38"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="43"/>
+      <c r="I5" s="55"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A6" s="55"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="69"/>
       <c r="D6" s="5">
         <v>3</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="38"/>
+      <c r="G6" s="55"/>
       <c r="H6" s="38"/>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A7" s="38"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="43"/>
+      <c r="I6" s="55"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A7" s="55"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="69"/>
       <c r="D7" s="5">
         <v>4</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="6"/>
-      <c r="G7" s="38"/>
+      <c r="G7" s="55"/>
       <c r="H7" s="38"/>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1">
+      <c r="I7" s="55"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1891,60 +1963,65 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A9" s="37" t="s">
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A9" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="42"/>
+      <c r="C9" s="68"/>
       <c r="D9" s="5">
         <v>1</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="6"/>
-      <c r="G9" s="37"/>
+      <c r="G9" s="54"/>
       <c r="H9" s="37"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A10" s="38"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="43"/>
+      <c r="I9" s="54"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A10" s="55"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="69"/>
       <c r="D10" s="5">
         <v>2</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="38"/>
+      <c r="G10" s="55"/>
       <c r="H10" s="38"/>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A11" s="38"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="43"/>
+      <c r="I10" s="55"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A11" s="55"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="69"/>
       <c r="D11" s="5">
         <v>3</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="38"/>
+      <c r="G11" s="55"/>
       <c r="H11" s="38"/>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A12" s="47"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="44"/>
+      <c r="I11" s="55"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A12" s="67"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="70"/>
       <c r="D12" s="5">
         <v>4</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1">
+      <c r="G12" s="67"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="67"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickBot="1">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1953,20 +2030,21 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:I1"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="B4:B7"/>
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="G4:G7"/>
-    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="I4:I7"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="B9:B12"/>
     <mergeCell ref="C9:C12"/>
     <mergeCell ref="G9:G12"/>
-    <mergeCell ref="H9:H12"/>
+    <mergeCell ref="I9:I12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1974,10 +2052,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1985,22 +2063,23 @@
     <col min="3" max="3" width="26.28515625" customWidth="1"/>
     <col min="5" max="5" width="29.140625" customWidth="1"/>
     <col min="6" max="6" width="22.28515625" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" customWidth="1"/>
+    <col min="7" max="8" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="36.75" customHeight="1" thickBot="1">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:9" ht="36.75" customHeight="1" thickBot="1">
+      <c r="A1" s="56" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2023,10 +2102,13 @@
         <v>6</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -2048,67 +2130,72 @@
       <c r="G3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="4"/>
+      <c r="I3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A4" s="37" t="s">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A4" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="74" t="s">
         <v>116</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="77" t="s">
         <v>123</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="48">
         <v>1</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="37" t="s">
+      <c r="E4" s="49"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="74" t="s">
         <v>124</v>
       </c>
-      <c r="H4" s="37"/>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A5" s="38"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="5">
+      <c r="H4" s="51"/>
+      <c r="I4" s="74"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A5" s="75"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="48">
         <v>2</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A6" s="38"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="5">
+      <c r="E5" s="49"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="75"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A6" s="75"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="48">
         <v>3</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A7" s="38"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="5">
+      <c r="E6" s="49"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="75"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A7" s="75"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="48">
         <v>4</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1">
+      <c r="E7" s="49"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="75"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -2117,60 +2204,65 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A9" s="37" t="s">
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A9" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="74" t="s">
         <v>117</v>
       </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="5">
+      <c r="C9" s="77"/>
+      <c r="D9" s="48">
         <v>1</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A10" s="38"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="5">
+      <c r="E9" s="49"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="74"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A10" s="75"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="48">
         <v>2</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A11" s="38"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="5">
+      <c r="E10" s="49"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="75"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A11" s="75"/>
+      <c r="B11" s="75"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="48">
         <v>3</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A12" s="47"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="5">
+      <c r="E11" s="49"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="75"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A12" s="76"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="79"/>
+      <c r="D12" s="48">
         <v>4</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1">
+      <c r="E12" s="49"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="76"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickBot="1">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -2179,20 +2271,21 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:I1"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="B4:B7"/>
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="G4:G7"/>
-    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="I4:I7"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="B9:B12"/>
     <mergeCell ref="C9:C12"/>
     <mergeCell ref="G9:G12"/>
-    <mergeCell ref="H9:H12"/>
+    <mergeCell ref="I9:I12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2200,10 +2293,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A4" sqref="A4:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2213,19 +2306,20 @@
     <col min="6" max="6" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="44.25" customHeight="1" thickBot="1">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:9" ht="44.25" customHeight="1" thickBot="1">
+      <c r="A1" s="56" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2248,10 +2342,13 @@
         <v>6</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -2273,18 +2370,19 @@
       <c r="G3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="4"/>
+      <c r="I3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="27" customHeight="1" thickBot="1">
-      <c r="A4" s="37" t="s">
+    <row r="4" spans="1:9" ht="27" customHeight="1" thickBot="1">
+      <c r="A4" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="57" t="s">
         <v>119</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="68" t="s">
         <v>122</v>
       </c>
       <c r="D4" s="5">
@@ -2296,13 +2394,14 @@
       <c r="F4" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="G4" s="37"/>
+      <c r="G4" s="54"/>
       <c r="H4" s="37"/>
-    </row>
-    <row r="5" spans="1:8" ht="42.75" customHeight="1" thickBot="1">
-      <c r="A5" s="38"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="43"/>
+      <c r="I4" s="54"/>
+    </row>
+    <row r="5" spans="1:9" ht="42.75" customHeight="1" thickBot="1">
+      <c r="A5" s="55"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="69"/>
       <c r="D5" s="5">
         <v>2</v>
       </c>
@@ -2312,13 +2411,14 @@
       <c r="F5" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="G5" s="38"/>
+      <c r="G5" s="55"/>
       <c r="H5" s="38"/>
-    </row>
-    <row r="6" spans="1:8" ht="27" customHeight="1" thickBot="1">
-      <c r="A6" s="38"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="43"/>
+      <c r="I5" s="55"/>
+    </row>
+    <row r="6" spans="1:9" ht="27" customHeight="1" thickBot="1">
+      <c r="A6" s="55"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="69"/>
       <c r="D6" s="5">
         <v>3</v>
       </c>
@@ -2328,13 +2428,14 @@
       <c r="F6" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="G6" s="38"/>
+      <c r="G6" s="55"/>
       <c r="H6" s="38"/>
-    </row>
-    <row r="7" spans="1:8" ht="31.5" customHeight="1" thickBot="1">
-      <c r="A7" s="38"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="43"/>
+      <c r="I6" s="55"/>
+    </row>
+    <row r="7" spans="1:9" ht="31.5" customHeight="1" thickBot="1">
+      <c r="A7" s="55"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="69"/>
       <c r="D7" s="5">
         <v>4</v>
       </c>
@@ -2344,10 +2445,11 @@
       <c r="F7" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="G7" s="38"/>
+      <c r="G7" s="55"/>
       <c r="H7" s="38"/>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1">
+      <c r="I7" s="55"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -2356,15 +2458,16 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A9" s="37" t="s">
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A9" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="57" t="s">
         <v>120</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="68" t="s">
         <v>134</v>
       </c>
       <c r="D9" s="5">
@@ -2372,46 +2475,50 @@
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="6"/>
-      <c r="G9" s="37"/>
+      <c r="G9" s="54"/>
       <c r="H9" s="37"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A10" s="38"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="43"/>
+      <c r="I9" s="54"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A10" s="55"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="69"/>
       <c r="D10" s="5">
         <v>2</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="38"/>
+      <c r="G10" s="55"/>
       <c r="H10" s="38"/>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A11" s="38"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="43"/>
+      <c r="I10" s="55"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A11" s="55"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="69"/>
       <c r="D11" s="5">
         <v>3</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="38"/>
+      <c r="G11" s="55"/>
       <c r="H11" s="38"/>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A12" s="47"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="44"/>
+      <c r="I11" s="55"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A12" s="67"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="70"/>
       <c r="D12" s="5">
         <v>4</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1">
+      <c r="G12" s="67"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="67"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickBot="1">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -2420,20 +2527,21 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:I1"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="B4:B7"/>
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="G4:G7"/>
-    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="I4:I7"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="B9:B12"/>
     <mergeCell ref="C9:C12"/>
     <mergeCell ref="G9:G12"/>
-    <mergeCell ref="H9:H12"/>
+    <mergeCell ref="I9:I12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2443,14 +2551,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView topLeftCell="B23" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31:C34"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="3" max="3" width="35.5703125" style="62" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" style="45" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" customWidth="1"/>
     <col min="5" max="5" width="33.28515625" customWidth="1"/>
     <col min="6" max="6" width="27.85546875" customWidth="1"/>
@@ -2459,17 +2567,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="41.25" customHeight="1" thickBot="1">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
     </row>
     <row r="2" spans="1:9" ht="18.75" thickBot="1">
       <c r="A2" s="1" t="s">
@@ -2478,7 +2586,7 @@
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="55" t="s">
+      <c r="C2" s="41" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -2505,7 +2613,7 @@
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="42" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -2528,13 +2636,13 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="62.25" customHeight="1" thickBot="1">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="57" t="s">
+      <c r="C4" s="59" t="s">
         <v>130</v>
       </c>
       <c r="D4" s="5">
@@ -2546,16 +2654,16 @@
       <c r="F4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="52" t="s">
+      <c r="G4" s="62" t="s">
         <v>128</v>
       </c>
       <c r="H4" s="30"/>
-      <c r="I4" s="37"/>
+      <c r="I4" s="54"/>
     </row>
     <row r="5" spans="1:9" ht="69" customHeight="1" thickBot="1">
-      <c r="A5" s="38"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="58"/>
+      <c r="A5" s="55"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="60"/>
       <c r="D5" s="5">
         <v>2</v>
       </c>
@@ -2565,14 +2673,14 @@
       <c r="F5" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="53"/>
+      <c r="G5" s="63"/>
       <c r="H5" s="31"/>
-      <c r="I5" s="38"/>
+      <c r="I5" s="55"/>
     </row>
     <row r="6" spans="1:9" ht="69" customHeight="1" thickBot="1">
-      <c r="A6" s="38"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="58"/>
+      <c r="A6" s="55"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="60"/>
       <c r="D6" s="5">
         <v>3</v>
       </c>
@@ -2582,14 +2690,14 @@
       <c r="F6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="53"/>
+      <c r="G6" s="63"/>
       <c r="H6" s="31"/>
-      <c r="I6" s="38"/>
+      <c r="I6" s="55"/>
     </row>
     <row r="7" spans="1:9" ht="115.5" customHeight="1" thickBot="1">
-      <c r="A7" s="38"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="58"/>
+      <c r="A7" s="55"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="60"/>
       <c r="D7" s="26">
         <v>4</v>
       </c>
@@ -2599,14 +2707,14 @@
       <c r="F7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="53"/>
+      <c r="G7" s="63"/>
       <c r="H7" s="31"/>
-      <c r="I7" s="38"/>
+      <c r="I7" s="55"/>
     </row>
     <row r="8" spans="1:9" ht="69" customHeight="1" thickBot="1">
       <c r="A8" s="17"/>
       <c r="B8" s="18"/>
-      <c r="C8" s="59"/>
+      <c r="C8" s="43"/>
       <c r="D8" s="12">
         <v>5</v>
       </c>
@@ -2616,14 +2724,14 @@
       <c r="F8" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="53"/>
+      <c r="G8" s="63"/>
       <c r="H8" s="31"/>
       <c r="I8" s="17"/>
     </row>
     <row r="9" spans="1:9" ht="69" customHeight="1" thickBot="1">
       <c r="A9" s="17"/>
       <c r="B9" s="18"/>
-      <c r="C9" s="59"/>
+      <c r="C9" s="43"/>
       <c r="D9" s="12">
         <v>6</v>
       </c>
@@ -2633,14 +2741,14 @@
       <c r="F9" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="53"/>
+      <c r="G9" s="63"/>
       <c r="H9" s="31"/>
       <c r="I9" s="17"/>
     </row>
     <row r="10" spans="1:9" ht="69" customHeight="1" thickBot="1">
       <c r="A10" s="17"/>
       <c r="B10" s="18"/>
-      <c r="C10" s="59"/>
+      <c r="C10" s="43"/>
       <c r="D10" s="12">
         <v>7</v>
       </c>
@@ -2650,14 +2758,14 @@
       <c r="F10" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="53"/>
+      <c r="G10" s="63"/>
       <c r="H10" s="31"/>
       <c r="I10" s="17"/>
     </row>
     <row r="11" spans="1:9" ht="69" customHeight="1" thickBot="1">
       <c r="A11" s="17"/>
       <c r="B11" s="18"/>
-      <c r="C11" s="59"/>
+      <c r="C11" s="43"/>
       <c r="D11" s="12">
         <v>8</v>
       </c>
@@ -2667,7 +2775,7 @@
       <c r="F11" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="G11" s="54"/>
+      <c r="G11" s="64"/>
       <c r="H11" s="32" t="s">
         <v>53</v>
       </c>
@@ -2676,7 +2784,7 @@
     <row r="12" spans="1:9" ht="15.75" thickBot="1">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
-      <c r="C12" s="56"/>
+      <c r="C12" s="42"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="27"/>
@@ -2685,13 +2793,13 @@
       <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:9" ht="39.75" customHeight="1" thickBot="1">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="57" t="s">
+      <c r="C13" s="59" t="s">
         <v>131</v>
       </c>
       <c r="D13" s="5">
@@ -2703,18 +2811,18 @@
       <c r="F13" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="37" t="s">
+      <c r="G13" s="54" t="s">
         <v>13</v>
       </c>
       <c r="H13" s="16"/>
-      <c r="I13" s="37" t="s">
+      <c r="I13" s="54" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="72.75" customHeight="1" thickBot="1">
-      <c r="A14" s="38"/>
-      <c r="B14" s="41"/>
-      <c r="C14" s="58"/>
+      <c r="A14" s="55"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="60"/>
       <c r="D14" s="5">
         <v>2</v>
       </c>
@@ -2724,14 +2832,14 @@
       <c r="F14" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="38"/>
+      <c r="G14" s="55"/>
       <c r="H14" s="17"/>
-      <c r="I14" s="38"/>
+      <c r="I14" s="55"/>
     </row>
     <row r="15" spans="1:9" ht="96" customHeight="1" thickBot="1">
-      <c r="A15" s="38"/>
-      <c r="B15" s="41"/>
-      <c r="C15" s="58"/>
+      <c r="A15" s="55"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="60"/>
       <c r="D15" s="5">
         <v>3</v>
       </c>
@@ -2741,14 +2849,14 @@
       <c r="F15" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G15" s="38"/>
+      <c r="G15" s="55"/>
       <c r="H15" s="17"/>
-      <c r="I15" s="38"/>
+      <c r="I15" s="55"/>
     </row>
     <row r="16" spans="1:9" ht="96" customHeight="1" thickBot="1">
       <c r="A16" s="17"/>
       <c r="B16" s="18"/>
-      <c r="C16" s="58"/>
+      <c r="C16" s="60"/>
       <c r="D16" s="5">
         <v>4</v>
       </c>
@@ -2765,7 +2873,7 @@
     <row r="17" spans="1:9" ht="122.25" customHeight="1" thickBot="1">
       <c r="A17" s="17"/>
       <c r="B17" s="18"/>
-      <c r="C17" s="58"/>
+      <c r="C17" s="60"/>
       <c r="D17" s="5">
         <v>5</v>
       </c>
@@ -2784,7 +2892,7 @@
     <row r="18" spans="1:9" ht="29.25" customHeight="1" thickBot="1">
       <c r="A18" s="10"/>
       <c r="B18" s="11"/>
-      <c r="C18" s="60"/>
+      <c r="C18" s="61"/>
       <c r="D18" s="5">
         <v>4</v>
       </c>
@@ -2797,7 +2905,7 @@
     <row r="19" spans="1:9" ht="15.75" thickBot="1">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
-      <c r="C19" s="56"/>
+      <c r="C19" s="42"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -2806,13 +2914,13 @@
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9" ht="32.25" customHeight="1" thickBot="1">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="57" t="s">
+      <c r="C20" s="59" t="s">
         <v>59</v>
       </c>
       <c r="D20" s="5">
@@ -2824,18 +2932,18 @@
       <c r="F20" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G20" s="45" t="s">
+      <c r="G20" s="65" t="s">
         <v>13</v>
       </c>
       <c r="H20" s="16"/>
-      <c r="I20" s="37" t="s">
+      <c r="I20" s="54" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="32.25" thickBot="1">
-      <c r="A21" s="38"/>
-      <c r="B21" s="41"/>
-      <c r="C21" s="58"/>
+      <c r="A21" s="55"/>
+      <c r="B21" s="58"/>
+      <c r="C21" s="60"/>
       <c r="D21" s="5">
         <v>2</v>
       </c>
@@ -2845,14 +2953,14 @@
       <c r="F21" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G21" s="46"/>
+      <c r="G21" s="66"/>
       <c r="H21" s="17"/>
-      <c r="I21" s="38"/>
+      <c r="I21" s="55"/>
     </row>
     <row r="22" spans="1:9" ht="63.75" thickBot="1">
-      <c r="A22" s="38"/>
-      <c r="B22" s="41"/>
-      <c r="C22" s="58"/>
+      <c r="A22" s="55"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="60"/>
       <c r="D22" s="5">
         <v>3</v>
       </c>
@@ -2862,14 +2970,14 @@
       <c r="F22" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="G22" s="46"/>
+      <c r="G22" s="66"/>
       <c r="H22" s="17"/>
-      <c r="I22" s="38"/>
+      <c r="I22" s="55"/>
     </row>
     <row r="23" spans="1:9" ht="41.25" customHeight="1" thickBot="1">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
-      <c r="C23" s="60"/>
+      <c r="C23" s="61"/>
       <c r="D23" s="5"/>
       <c r="E23" s="7"/>
       <c r="F23" s="25"/>
@@ -2880,7 +2988,7 @@
     <row r="24" spans="1:9" ht="15.75" thickBot="1">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
-      <c r="C24" s="56"/>
+      <c r="C24" s="42"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -2889,13 +2997,13 @@
       <c r="I24" s="3"/>
     </row>
     <row r="25" spans="1:9" ht="32.25" thickBot="1">
-      <c r="A25" s="37" t="s">
+      <c r="A25" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="40" t="s">
+      <c r="B25" s="57" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="57" t="s">
+      <c r="C25" s="59" t="s">
         <v>32</v>
       </c>
       <c r="D25" s="5">
@@ -2907,16 +3015,16 @@
       <c r="F25" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="G25" s="37"/>
+      <c r="G25" s="54"/>
       <c r="H25" s="16"/>
-      <c r="I25" s="37" t="s">
+      <c r="I25" s="54" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="39" customHeight="1" thickBot="1">
-      <c r="A26" s="38"/>
-      <c r="B26" s="41"/>
-      <c r="C26" s="58"/>
+      <c r="A26" s="55"/>
+      <c r="B26" s="58"/>
+      <c r="C26" s="60"/>
       <c r="D26" s="5">
         <v>2</v>
       </c>
@@ -2926,14 +3034,14 @@
       <c r="F26" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="G26" s="38"/>
+      <c r="G26" s="55"/>
       <c r="H26" s="17"/>
-      <c r="I26" s="38"/>
+      <c r="I26" s="55"/>
     </row>
     <row r="27" spans="1:9" ht="37.5" customHeight="1" thickBot="1">
-      <c r="A27" s="38"/>
-      <c r="B27" s="41"/>
-      <c r="C27" s="58"/>
+      <c r="A27" s="55"/>
+      <c r="B27" s="58"/>
+      <c r="C27" s="60"/>
       <c r="D27" s="5">
         <v>3</v>
       </c>
@@ -2943,16 +3051,16 @@
       <c r="F27" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="G27" s="38"/>
+      <c r="G27" s="55"/>
       <c r="H27" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="I27" s="38"/>
+      <c r="I27" s="55"/>
     </row>
     <row r="28" spans="1:9" ht="44.25" customHeight="1" thickBot="1">
       <c r="A28" s="10"/>
       <c r="B28" s="11"/>
-      <c r="C28" s="60"/>
+      <c r="C28" s="61"/>
       <c r="D28" s="5">
         <v>4</v>
       </c>
@@ -2969,7 +3077,7 @@
     <row r="29" spans="1:9" ht="30.75" customHeight="1" thickBot="1">
       <c r="A29" s="17"/>
       <c r="B29" s="18"/>
-      <c r="C29" s="61"/>
+      <c r="C29" s="44"/>
       <c r="D29" s="5">
         <v>5</v>
       </c>
@@ -2988,7 +3096,7 @@
     <row r="30" spans="1:9" ht="15.75" thickBot="1">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
-      <c r="C30" s="56"/>
+      <c r="C30" s="42"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -2997,13 +3105,13 @@
       <c r="I30" s="3"/>
     </row>
     <row r="31" spans="1:9" ht="32.25" thickBot="1">
-      <c r="A31" s="37" t="s">
+      <c r="A31" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="40" t="s">
+      <c r="B31" s="57" t="s">
         <v>127</v>
       </c>
-      <c r="C31" s="57" t="s">
+      <c r="C31" s="59" t="s">
         <v>78</v>
       </c>
       <c r="D31" s="5">
@@ -3015,16 +3123,16 @@
       <c r="F31" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="G31" s="37"/>
+      <c r="G31" s="54"/>
       <c r="H31" s="16"/>
-      <c r="I31" s="37" t="s">
+      <c r="I31" s="54" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="21.75" thickBot="1">
-      <c r="A32" s="38"/>
-      <c r="B32" s="41"/>
-      <c r="C32" s="58"/>
+      <c r="A32" s="55"/>
+      <c r="B32" s="58"/>
+      <c r="C32" s="60"/>
       <c r="D32" s="5">
         <v>2</v>
       </c>
@@ -3034,14 +3142,14 @@
       <c r="F32" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="G32" s="38"/>
+      <c r="G32" s="55"/>
       <c r="H32" s="17"/>
-      <c r="I32" s="38"/>
+      <c r="I32" s="55"/>
     </row>
     <row r="33" spans="1:9" ht="32.25" thickBot="1">
-      <c r="A33" s="38"/>
-      <c r="B33" s="41"/>
-      <c r="C33" s="58"/>
+      <c r="A33" s="55"/>
+      <c r="B33" s="58"/>
+      <c r="C33" s="60"/>
       <c r="D33" s="5">
         <v>3</v>
       </c>
@@ -3051,14 +3159,14 @@
       <c r="F33" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="G33" s="38"/>
+      <c r="G33" s="55"/>
       <c r="H33" s="17"/>
-      <c r="I33" s="38"/>
+      <c r="I33" s="55"/>
     </row>
     <row r="34" spans="1:9" ht="95.25" thickBot="1">
       <c r="A34" s="10"/>
       <c r="B34" s="11"/>
-      <c r="C34" s="60"/>
+      <c r="C34" s="61"/>
       <c r="D34" s="5">
         <v>4</v>
       </c>
@@ -3075,7 +3183,7 @@
     <row r="35" spans="1:9" ht="95.25" thickBot="1">
       <c r="A35" s="17"/>
       <c r="B35" s="18"/>
-      <c r="C35" s="61"/>
+      <c r="C35" s="44"/>
       <c r="D35" s="5">
         <v>5</v>
       </c>
@@ -3094,7 +3202,7 @@
     <row r="36" spans="1:9" ht="15.75" thickBot="1">
       <c r="A36" s="17"/>
       <c r="B36" s="18"/>
-      <c r="C36" s="61"/>
+      <c r="C36" s="44"/>
       <c r="D36" s="5"/>
       <c r="E36" s="33"/>
       <c r="F36" s="34"/>
@@ -3105,7 +3213,7 @@
     <row r="37" spans="1:9" ht="15.75" thickBot="1">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
-      <c r="C37" s="56"/>
+      <c r="C37" s="42"/>
       <c r="D37" s="3"/>
       <c r="E37" s="27"/>
       <c r="F37" s="27"/>
@@ -3114,56 +3222,56 @@
       <c r="I37" s="3"/>
     </row>
     <row r="38" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A38" s="37" t="s">
+      <c r="A38" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B38" s="40" t="s">
+      <c r="B38" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="57"/>
+      <c r="C38" s="59"/>
       <c r="D38" s="5">
         <v>1</v>
       </c>
       <c r="E38" s="7"/>
       <c r="F38" s="6"/>
-      <c r="G38" s="37" t="s">
+      <c r="G38" s="54" t="s">
         <v>13</v>
       </c>
       <c r="H38" s="16"/>
-      <c r="I38" s="37" t="s">
+      <c r="I38" s="54" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A39" s="38"/>
-      <c r="B39" s="41"/>
-      <c r="C39" s="58"/>
+      <c r="A39" s="55"/>
+      <c r="B39" s="58"/>
+      <c r="C39" s="60"/>
       <c r="D39" s="5">
         <v>2</v>
       </c>
       <c r="E39" s="7"/>
       <c r="F39" s="6"/>
-      <c r="G39" s="38"/>
+      <c r="G39" s="55"/>
       <c r="H39" s="17"/>
-      <c r="I39" s="38"/>
+      <c r="I39" s="55"/>
     </row>
     <row r="40" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A40" s="38"/>
-      <c r="B40" s="41"/>
-      <c r="C40" s="58"/>
+      <c r="A40" s="55"/>
+      <c r="B40" s="58"/>
+      <c r="C40" s="60"/>
       <c r="D40" s="5">
         <v>3</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="6"/>
-      <c r="G40" s="38"/>
+      <c r="G40" s="55"/>
       <c r="H40" s="17"/>
-      <c r="I40" s="38"/>
+      <c r="I40" s="55"/>
     </row>
     <row r="41" spans="1:9" ht="15.75" thickBot="1">
       <c r="A41" s="10"/>
       <c r="B41" s="11"/>
-      <c r="C41" s="60"/>
+      <c r="C41" s="61"/>
       <c r="D41" s="5">
         <v>4</v>
       </c>
@@ -3176,7 +3284,7 @@
     <row r="42" spans="1:9" ht="15.75" thickBot="1">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
-      <c r="C42" s="56"/>
+      <c r="C42" s="42"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
@@ -3185,10 +3293,10 @@
       <c r="I42" s="3"/>
     </row>
     <row r="43" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A43" s="37" t="s">
+      <c r="A43" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B43" s="40" t="s">
+      <c r="B43" s="57" t="s">
         <v>28</v>
       </c>
       <c r="D43" s="5">
@@ -3196,37 +3304,37 @@
       </c>
       <c r="E43" s="7"/>
       <c r="F43" s="6"/>
-      <c r="G43" s="37" t="s">
+      <c r="G43" s="54" t="s">
         <v>13</v>
       </c>
       <c r="H43" s="16"/>
-      <c r="I43" s="37" t="s">
+      <c r="I43" s="54" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A44" s="38"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="55"/>
+      <c r="B44" s="58"/>
       <c r="D44" s="5">
         <v>2</v>
       </c>
       <c r="E44" s="7"/>
       <c r="F44" s="6"/>
-      <c r="G44" s="38"/>
+      <c r="G44" s="55"/>
       <c r="H44" s="17"/>
-      <c r="I44" s="38"/>
+      <c r="I44" s="55"/>
     </row>
     <row r="45" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A45" s="38"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="55"/>
+      <c r="B45" s="58"/>
       <c r="D45" s="5">
         <v>3</v>
       </c>
       <c r="E45" s="7"/>
       <c r="F45" s="6"/>
-      <c r="G45" s="38"/>
+      <c r="G45" s="55"/>
       <c r="H45" s="17"/>
-      <c r="I45" s="38"/>
+      <c r="I45" s="55"/>
     </row>
     <row r="46" spans="1:9" ht="15.75" thickBot="1">
       <c r="A46" s="10"/>
@@ -3243,7 +3351,7 @@
     <row r="47" spans="1:9" ht="15.75" thickBot="1">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
-      <c r="C47" s="56"/>
+      <c r="C47" s="42"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
@@ -3302,10 +3410,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C10"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3316,19 +3424,20 @@
     <col min="6" max="6" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="36.75" customHeight="1" thickBot="1">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:10" ht="36.75" customHeight="1" thickBot="1">
+      <c r="A1" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-    </row>
-    <row r="2" spans="1:9" ht="18.75" thickBot="1">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3350,11 +3459,12 @@
       <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="2"/>
+      <c r="I2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -3377,17 +3487,20 @@
         <v>6</v>
       </c>
       <c r="H3" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A4" s="37" t="s">
+    <row r="4" spans="1:10" ht="33.75" customHeight="1" thickBot="1">
+      <c r="A4" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="68" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="68" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="5">
@@ -3399,15 +3512,16 @@
       <c r="F4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="37" t="s">
+      <c r="G4" s="54" t="s">
         <v>52</v>
       </c>
       <c r="H4" s="37"/>
-    </row>
-    <row r="5" spans="1:9" ht="45.75" customHeight="1" thickBot="1">
-      <c r="A5" s="38"/>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
+      <c r="I4" s="54"/>
+    </row>
+    <row r="5" spans="1:10" ht="45.75" customHeight="1" thickBot="1">
+      <c r="A5" s="55"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
       <c r="D5" s="5">
         <v>2</v>
       </c>
@@ -3417,13 +3531,14 @@
       <c r="F5" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="38"/>
+      <c r="G5" s="55"/>
       <c r="H5" s="38"/>
-    </row>
-    <row r="6" spans="1:9" ht="45.75" customHeight="1" thickBot="1">
-      <c r="A6" s="38"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
+      <c r="I5" s="55"/>
+    </row>
+    <row r="6" spans="1:10" ht="45.75" customHeight="1" thickBot="1">
+      <c r="A6" s="55"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="69"/>
       <c r="D6" s="5">
         <v>3</v>
       </c>
@@ -3433,13 +3548,14 @@
       <c r="F6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="38"/>
+      <c r="G6" s="55"/>
       <c r="H6" s="38"/>
-    </row>
-    <row r="7" spans="1:9" ht="95.25" thickBot="1">
-      <c r="A7" s="38"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
+      <c r="I6" s="55"/>
+    </row>
+    <row r="7" spans="1:10" ht="95.25" thickBot="1">
+      <c r="A7" s="55"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="69"/>
       <c r="D7" s="5">
         <v>4</v>
       </c>
@@ -3449,13 +3565,14 @@
       <c r="F7" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="G7" s="38"/>
+      <c r="G7" s="55"/>
       <c r="H7" s="38"/>
-    </row>
-    <row r="8" spans="1:9" ht="32.25" thickBot="1">
-      <c r="A8" s="38"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
+      <c r="I7" s="55"/>
+    </row>
+    <row r="8" spans="1:10" ht="32.25" thickBot="1">
+      <c r="A8" s="55"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="69"/>
       <c r="D8" s="5">
         <v>5</v>
       </c>
@@ -3465,13 +3582,14 @@
       <c r="F8" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="38"/>
+      <c r="G8" s="55"/>
       <c r="H8" s="38"/>
-    </row>
-    <row r="9" spans="1:9" ht="32.25" thickBot="1">
-      <c r="A9" s="38"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="43"/>
+      <c r="I8" s="55"/>
+    </row>
+    <row r="9" spans="1:10" ht="32.25" thickBot="1">
+      <c r="A9" s="55"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="69"/>
       <c r="D9" s="5">
         <v>6</v>
       </c>
@@ -3481,13 +3599,14 @@
       <c r="F9" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="38"/>
+      <c r="G9" s="55"/>
       <c r="H9" s="38"/>
-    </row>
-    <row r="10" spans="1:9" ht="32.25" thickBot="1">
-      <c r="A10" s="47"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
+      <c r="I9" s="55"/>
+    </row>
+    <row r="10" spans="1:10" ht="32.25" thickBot="1">
+      <c r="A10" s="67"/>
+      <c r="B10" s="70"/>
+      <c r="C10" s="70"/>
       <c r="D10" s="5">
         <v>7</v>
       </c>
@@ -3497,10 +3616,11 @@
       <c r="F10" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1">
+      <c r="G10" s="67"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="67"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -3509,16 +3629,17 @@
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
-      <c r="I11" s="9"/>
-    </row>
-    <row r="12" spans="1:9" ht="42.75" thickBot="1">
-      <c r="A12" s="37" t="s">
+      <c r="I11" s="8"/>
+      <c r="J11" s="9"/>
+    </row>
+    <row r="12" spans="1:10" ht="42.75" thickBot="1">
+      <c r="A12" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="68" t="s">
         <v>133</v>
       </c>
-      <c r="C12" s="42" t="s">
+      <c r="C12" s="68" t="s">
         <v>129</v>
       </c>
       <c r="D12" s="5">
@@ -3530,14 +3651,15 @@
       <c r="F12" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="37"/>
+      <c r="G12" s="54"/>
       <c r="H12" s="37"/>
-      <c r="I12" s="9"/>
-    </row>
-    <row r="13" spans="1:9" ht="48.75" customHeight="1" thickBot="1">
-      <c r="A13" s="38"/>
-      <c r="B13" s="43"/>
-      <c r="C13" s="43"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="9"/>
+    </row>
+    <row r="13" spans="1:10" ht="48.75" customHeight="1" thickBot="1">
+      <c r="A13" s="55"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="69"/>
       <c r="D13" s="5">
         <v>2</v>
       </c>
@@ -3547,14 +3669,15 @@
       <c r="F13" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G13" s="38"/>
+      <c r="G13" s="55"/>
       <c r="H13" s="38"/>
-      <c r="I13" s="9"/>
-    </row>
-    <row r="14" spans="1:9" ht="48.75" customHeight="1" thickBot="1">
-      <c r="A14" s="38"/>
-      <c r="B14" s="43"/>
-      <c r="C14" s="43"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="9"/>
+    </row>
+    <row r="14" spans="1:10" ht="48.75" customHeight="1" thickBot="1">
+      <c r="A14" s="55"/>
+      <c r="B14" s="69"/>
+      <c r="C14" s="69"/>
       <c r="D14" s="5">
         <v>3</v>
       </c>
@@ -3564,14 +3687,15 @@
       <c r="F14" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="38"/>
+      <c r="G14" s="55"/>
       <c r="H14" s="38"/>
-      <c r="I14" s="9"/>
-    </row>
-    <row r="15" spans="1:9" ht="120.75" customHeight="1" thickBot="1">
-      <c r="A15" s="38"/>
-      <c r="B15" s="43"/>
-      <c r="C15" s="43"/>
+      <c r="I14" s="55"/>
+      <c r="J14" s="9"/>
+    </row>
+    <row r="15" spans="1:10" ht="120.75" customHeight="1" thickBot="1">
+      <c r="A15" s="55"/>
+      <c r="B15" s="69"/>
+      <c r="C15" s="69"/>
       <c r="D15" s="5">
         <v>4</v>
       </c>
@@ -3581,14 +3705,15 @@
       <c r="F15" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="G15" s="38"/>
+      <c r="G15" s="55"/>
       <c r="H15" s="38"/>
-      <c r="I15" s="9"/>
-    </row>
-    <row r="16" spans="1:9" ht="42.75" customHeight="1" thickBot="1">
-      <c r="A16" s="47"/>
-      <c r="B16" s="44"/>
-      <c r="C16" s="44"/>
+      <c r="I15" s="55"/>
+      <c r="J15" s="9"/>
+    </row>
+    <row r="16" spans="1:10" ht="42.75" customHeight="1" thickBot="1">
+      <c r="A16" s="67"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="70"/>
       <c r="D16" s="5">
         <v>5</v>
       </c>
@@ -3598,11 +3723,12 @@
       <c r="F16" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="G16" s="47"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="9"/>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1">
+      <c r="G16" s="67"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="9"/>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" thickBot="1">
       <c r="A17" s="17"/>
       <c r="B17" s="20"/>
       <c r="C17" s="20"/>
@@ -3610,10 +3736,11 @@
       <c r="E17" s="24"/>
       <c r="F17" s="24"/>
       <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="9"/>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1">
+      <c r="H17" s="38"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="9"/>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" thickBot="1">
       <c r="A18" s="17"/>
       <c r="B18" s="20"/>
       <c r="C18" s="20"/>
@@ -3621,10 +3748,11 @@
       <c r="E18" s="24"/>
       <c r="F18" s="24"/>
       <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="9"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1">
+      <c r="H18" s="38"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="9"/>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" thickBot="1">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -3633,16 +3761,17 @@
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
-      <c r="I19" s="9"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A20" s="37" t="s">
+      <c r="I19" s="8"/>
+      <c r="J19" s="9"/>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A20" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="68" t="s">
         <v>35</v>
       </c>
       <c r="D20" s="5">
@@ -3650,34 +3779,37 @@
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="6"/>
-      <c r="G20" s="37"/>
+      <c r="G20" s="54"/>
       <c r="H20" s="37"/>
-      <c r="I20" s="9"/>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A21" s="38"/>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
+      <c r="I20" s="54"/>
+      <c r="J20" s="9"/>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A21" s="55"/>
+      <c r="B21" s="69"/>
+      <c r="C21" s="69"/>
       <c r="D21" s="5">
         <v>2</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="6"/>
-      <c r="G21" s="38"/>
+      <c r="G21" s="55"/>
       <c r="H21" s="38"/>
-      <c r="I21" s="9"/>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A22" s="47"/>
-      <c r="B22" s="44"/>
-      <c r="C22" s="44"/>
+      <c r="I21" s="55"/>
+      <c r="J21" s="9"/>
+    </row>
+    <row r="22" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A22" s="67"/>
+      <c r="B22" s="70"/>
+      <c r="C22" s="70"/>
       <c r="D22" s="5"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
-      <c r="G22" s="47"/>
-      <c r="H22" s="47"/>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="G22" s="67"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="67"/>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -3686,25 +3818,26 @@
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:I1"/>
     <mergeCell ref="A4:A10"/>
     <mergeCell ref="B4:B10"/>
     <mergeCell ref="C4:C10"/>
     <mergeCell ref="G4:G10"/>
-    <mergeCell ref="H4:H10"/>
+    <mergeCell ref="I4:I10"/>
     <mergeCell ref="A12:A16"/>
     <mergeCell ref="B12:B16"/>
     <mergeCell ref="C12:C16"/>
     <mergeCell ref="G12:G16"/>
-    <mergeCell ref="H12:H16"/>
+    <mergeCell ref="I12:I16"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="B20:B22"/>
     <mergeCell ref="C20:C22"/>
     <mergeCell ref="G20:G22"/>
-    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="I20:I22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3712,10 +3845,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3723,22 +3856,23 @@
     <col min="3" max="3" width="27.85546875" customWidth="1"/>
     <col min="5" max="5" width="25.140625" customWidth="1"/>
     <col min="6" max="6" width="31.28515625" customWidth="1"/>
-    <col min="8" max="8" width="31.5703125" customWidth="1"/>
+    <col min="9" max="9" width="31.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="39" customHeight="1" thickBot="1">
-      <c r="A1" s="48" t="s">
+    <row r="1" spans="1:9" ht="39" customHeight="1" thickBot="1">
+      <c r="A1" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1">
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3761,10 +3895,13 @@
         <v>6</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -3786,18 +3923,19 @@
       <c r="G3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="4"/>
+      <c r="I3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A4" s="37" t="s">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A4" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="68" t="s">
         <v>84</v>
       </c>
       <c r="D4" s="5">
@@ -3805,46 +3943,50 @@
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="6"/>
-      <c r="G4" s="37"/>
+      <c r="G4" s="54"/>
       <c r="H4" s="37"/>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A5" s="38"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="43"/>
+      <c r="I4" s="54"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A5" s="55"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="69"/>
       <c r="D5" s="5">
         <v>2</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="6"/>
-      <c r="G5" s="38"/>
+      <c r="G5" s="55"/>
       <c r="H5" s="38"/>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1">
+      <c r="I5" s="55"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1">
       <c r="A6" s="14"/>
       <c r="B6" s="15"/>
-      <c r="C6" s="43"/>
+      <c r="C6" s="69"/>
       <c r="D6" s="13">
         <v>3</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="24"/>
       <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1">
+      <c r="H6" s="38"/>
+      <c r="I6" s="14"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" thickBot="1">
       <c r="A7" s="14"/>
       <c r="B7" s="15"/>
-      <c r="C7" s="44"/>
+      <c r="C7" s="70"/>
       <c r="D7" s="13">
         <v>4</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="24"/>
       <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-    </row>
-    <row r="8" spans="1:8" ht="12.75" customHeight="1" thickBot="1">
+      <c r="H7" s="38"/>
+      <c r="I7" s="14"/>
+    </row>
+    <row r="8" spans="1:9" ht="12.75" customHeight="1" thickBot="1">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -3853,15 +3995,16 @@
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A9" s="37" t="s">
+      <c r="I8" s="8"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A9" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="68" t="s">
         <v>37</v>
       </c>
       <c r="D9" s="5">
@@ -3869,46 +4012,50 @@
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="6"/>
-      <c r="G9" s="37"/>
+      <c r="G9" s="54"/>
       <c r="H9" s="37"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A10" s="38"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="43"/>
+      <c r="I9" s="54"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A10" s="55"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="69"/>
       <c r="D10" s="5">
         <v>2</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="38"/>
+      <c r="G10" s="55"/>
       <c r="H10" s="38"/>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1">
+      <c r="I10" s="55"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" thickBot="1">
       <c r="A11" s="14"/>
       <c r="B11" s="15"/>
-      <c r="C11" s="43"/>
+      <c r="C11" s="69"/>
       <c r="D11" s="13">
         <v>3</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="24"/>
       <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1">
+      <c r="H11" s="38"/>
+      <c r="I11" s="14"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" thickBot="1">
       <c r="A12" s="14"/>
       <c r="B12" s="15"/>
-      <c r="C12" s="44"/>
+      <c r="C12" s="70"/>
       <c r="D12" s="13">
         <v>4</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="24"/>
       <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1">
+      <c r="H12" s="38"/>
+      <c r="I12" s="14"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickBot="1">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -3917,15 +4064,16 @@
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A14" s="37" t="s">
+      <c r="I13" s="8"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A14" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="68" t="s">
         <v>37</v>
       </c>
       <c r="D14" s="5">
@@ -3933,46 +4081,50 @@
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="6"/>
-      <c r="G14" s="37"/>
+      <c r="G14" s="54"/>
       <c r="H14" s="37"/>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A15" s="38"/>
-      <c r="B15" s="41"/>
-      <c r="C15" s="43"/>
+      <c r="I14" s="54"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A15" s="55"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="69"/>
       <c r="D15" s="5">
         <v>2</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="6"/>
-      <c r="G15" s="38"/>
+      <c r="G15" s="55"/>
       <c r="H15" s="38"/>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" thickBot="1">
+      <c r="I15" s="55"/>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" thickBot="1">
       <c r="A16" s="14"/>
       <c r="B16" s="15"/>
-      <c r="C16" s="43"/>
+      <c r="C16" s="69"/>
       <c r="D16" s="13">
         <v>3</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="24"/>
       <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" thickBot="1">
+      <c r="H16" s="38"/>
+      <c r="I16" s="14"/>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" thickBot="1">
       <c r="A17" s="14"/>
       <c r="B17" s="15"/>
-      <c r="C17" s="44"/>
+      <c r="C17" s="70"/>
       <c r="D17" s="13">
         <v>4</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="24"/>
       <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="H17" s="38"/>
+      <c r="I17" s="14"/>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -3981,25 +4133,26 @@
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:I1"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:I5"/>
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="C9:C12"/>
     <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:C17"/>
     <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I14:I15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4007,10 +4160,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4020,19 +4173,20 @@
     <col min="6" max="6" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A1" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -4055,10 +4209,13 @@
         <v>6</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -4080,18 +4237,19 @@
       <c r="G3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="4"/>
+      <c r="I3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="32.25" thickBot="1">
-      <c r="A4" s="37" t="s">
+    <row r="4" spans="1:9" ht="32.25" thickBot="1">
+      <c r="A4" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="68" t="s">
         <v>85</v>
       </c>
       <c r="D4" s="5">
@@ -4103,13 +4261,14 @@
       <c r="F4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="37"/>
+      <c r="G4" s="54"/>
       <c r="H4" s="37"/>
-    </row>
-    <row r="5" spans="1:8" ht="32.25" thickBot="1">
-      <c r="A5" s="38"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="43"/>
+      <c r="I4" s="54"/>
+    </row>
+    <row r="5" spans="1:9" ht="32.25" thickBot="1">
+      <c r="A5" s="55"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="69"/>
       <c r="D5" s="5">
         <v>2</v>
       </c>
@@ -4119,13 +4278,14 @@
       <c r="F5" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="G5" s="38"/>
+      <c r="G5" s="55"/>
       <c r="H5" s="38"/>
-    </row>
-    <row r="6" spans="1:8" ht="32.25" thickBot="1">
-      <c r="A6" s="38"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="43"/>
+      <c r="I5" s="55"/>
+    </row>
+    <row r="6" spans="1:9" ht="32.25" thickBot="1">
+      <c r="A6" s="55"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="69"/>
       <c r="D6" s="5">
         <v>3</v>
       </c>
@@ -4135,13 +4295,14 @@
       <c r="F6" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="G6" s="38"/>
+      <c r="G6" s="55"/>
       <c r="H6" s="38"/>
-    </row>
-    <row r="7" spans="1:8" ht="53.25" thickBot="1">
-      <c r="A7" s="47"/>
-      <c r="B7" s="49"/>
-      <c r="C7" s="44"/>
+      <c r="I6" s="55"/>
+    </row>
+    <row r="7" spans="1:9" ht="53.25" thickBot="1">
+      <c r="A7" s="67"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="70"/>
       <c r="D7" s="5">
         <v>4</v>
       </c>
@@ -4151,10 +4312,11 @@
       <c r="F7" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1">
+      <c r="G7" s="67"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="67"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="21"/>
@@ -4162,9 +4324,10 @@
       <c r="E8" s="7"/>
       <c r="F8" s="6"/>
       <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1">
+      <c r="H8" s="39"/>
+      <c r="I8" s="22"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1">
       <c r="A9" s="22"/>
       <c r="B9" s="23"/>
       <c r="C9" s="21"/>
@@ -4172,9 +4335,10 @@
       <c r="E9" s="7"/>
       <c r="F9" s="6"/>
       <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-    </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" thickBot="1">
+      <c r="H9" s="39"/>
+      <c r="I9" s="22"/>
+    </row>
+    <row r="10" spans="1:9" ht="15" customHeight="1" thickBot="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -4183,15 +4347,16 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:I1"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="B4:B7"/>
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="G4:G7"/>
-    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="I4:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4199,10 +4364,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:H7"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4212,19 +4377,20 @@
     <col min="6" max="6" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="53.25" customHeight="1" thickBot="1">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:9" ht="53.25" customHeight="1" thickBot="1">
+      <c r="A1" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -4247,10 +4413,13 @@
         <v>6</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -4272,18 +4441,19 @@
       <c r="G3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="4"/>
+      <c r="I3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="32.25" thickBot="1">
-      <c r="A4" s="37" t="s">
+    <row r="4" spans="1:9" ht="32.25" thickBot="1">
+      <c r="A4" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="68" t="s">
         <v>94</v>
       </c>
       <c r="D4" s="5">
@@ -4295,13 +4465,14 @@
       <c r="F4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="37"/>
+      <c r="G4" s="54"/>
       <c r="H4" s="37"/>
-    </row>
-    <row r="5" spans="1:8" ht="32.25" thickBot="1">
-      <c r="A5" s="38"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="43"/>
+      <c r="I4" s="54"/>
+    </row>
+    <row r="5" spans="1:9" ht="32.25" thickBot="1">
+      <c r="A5" s="55"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="69"/>
       <c r="D5" s="5">
         <v>2</v>
       </c>
@@ -4311,13 +4482,14 @@
       <c r="F5" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="G5" s="38"/>
+      <c r="G5" s="55"/>
       <c r="H5" s="38"/>
-    </row>
-    <row r="6" spans="1:8" ht="42.75" thickBot="1">
-      <c r="A6" s="38"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="43"/>
+      <c r="I5" s="55"/>
+    </row>
+    <row r="6" spans="1:9" ht="42.75" thickBot="1">
+      <c r="A6" s="55"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="69"/>
       <c r="D6" s="5">
         <v>3</v>
       </c>
@@ -4327,13 +4499,14 @@
       <c r="F6" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="G6" s="38"/>
+      <c r="G6" s="55"/>
       <c r="H6" s="38"/>
-    </row>
-    <row r="7" spans="1:8" ht="21.75" thickBot="1">
-      <c r="A7" s="38"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="43"/>
+      <c r="I6" s="55"/>
+    </row>
+    <row r="7" spans="1:9" ht="21.75" thickBot="1">
+      <c r="A7" s="55"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="69"/>
       <c r="D7" s="5">
         <v>4</v>
       </c>
@@ -4343,10 +4516,11 @@
       <c r="F7" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="G7" s="38"/>
+      <c r="G7" s="55"/>
       <c r="H7" s="38"/>
-    </row>
-    <row r="8" spans="1:8" ht="32.25" thickBot="1">
+      <c r="I7" s="55"/>
+    </row>
+    <row r="8" spans="1:9" ht="32.25" thickBot="1">
       <c r="A8" s="17"/>
       <c r="B8" s="18"/>
       <c r="C8" s="20"/>
@@ -4362,9 +4536,10 @@
       <c r="G8" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="17"/>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1">
+      <c r="H8" s="38"/>
+      <c r="I8" s="17"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -4373,52 +4548,57 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A10" s="37" t="s">
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A10" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="57" t="s">
         <v>93</v>
       </c>
-      <c r="C10" s="42"/>
+      <c r="C10" s="68"/>
       <c r="D10" s="5"/>
       <c r="E10" s="7"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="37"/>
+      <c r="G10" s="54"/>
       <c r="H10" s="37"/>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A11" s="38"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="43"/>
+      <c r="I10" s="54"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A11" s="55"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="69"/>
       <c r="D11" s="5"/>
       <c r="E11" s="7"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="38"/>
+      <c r="G11" s="55"/>
       <c r="H11" s="38"/>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A12" s="38"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="43"/>
+      <c r="I11" s="55"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A12" s="55"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="69"/>
       <c r="D12" s="5"/>
       <c r="E12" s="7"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="38"/>
+      <c r="G12" s="55"/>
       <c r="H12" s="38"/>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A13" s="47"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="44"/>
+      <c r="I12" s="55"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A13" s="67"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="70"/>
       <c r="D13" s="5"/>
       <c r="E13" s="7"/>
       <c r="F13" s="6"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47"/>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" thickBot="1">
+      <c r="G13" s="67"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="67"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -4427,6 +4607,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -4434,13 +4615,13 @@
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="C10:C13"/>
     <mergeCell ref="G10:G13"/>
-    <mergeCell ref="H10:H13"/>
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="I10:I13"/>
+    <mergeCell ref="A1:I1"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="B4:B7"/>
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="G4:G7"/>
-    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="I4:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4448,10 +4629,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4461,19 +4642,20 @@
     <col min="6" max="6" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="36" customHeight="1" thickBot="1">
-      <c r="A1" s="48" t="s">
+    <row r="1" spans="1:9" ht="36" customHeight="1" thickBot="1">
+      <c r="A1" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1">
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -4496,10 +4678,13 @@
         <v>6</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -4521,63 +4706,68 @@
       <c r="G3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="4"/>
+      <c r="I3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A4" s="37" t="s">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A4" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="57" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="42"/>
+      <c r="C4" s="68"/>
       <c r="D4" s="5">
         <v>1</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="6"/>
-      <c r="G4" s="37"/>
+      <c r="G4" s="54"/>
       <c r="H4" s="37"/>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A5" s="38"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="43"/>
+      <c r="I4" s="54"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A5" s="55"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="69"/>
       <c r="D5" s="5">
         <v>2</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="6"/>
-      <c r="G5" s="38"/>
+      <c r="G5" s="55"/>
       <c r="H5" s="38"/>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A6" s="38"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="43"/>
+      <c r="I5" s="55"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A6" s="55"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="69"/>
       <c r="D6" s="5">
         <v>3</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="38"/>
+      <c r="G6" s="55"/>
       <c r="H6" s="38"/>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A7" s="38"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="43"/>
+      <c r="I6" s="55"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A7" s="55"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="69"/>
       <c r="D7" s="5">
         <v>4</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="6"/>
-      <c r="G7" s="38"/>
+      <c r="G7" s="55"/>
       <c r="H7" s="38"/>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1">
+      <c r="I7" s="55"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -4586,60 +4776,65 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A9" s="37" t="s">
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A9" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="42"/>
+      <c r="C9" s="68"/>
       <c r="D9" s="5">
         <v>1</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="6"/>
-      <c r="G9" s="37"/>
+      <c r="G9" s="54"/>
       <c r="H9" s="37"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A10" s="38"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="43"/>
+      <c r="I9" s="54"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A10" s="55"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="69"/>
       <c r="D10" s="5">
         <v>2</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="38"/>
+      <c r="G10" s="55"/>
       <c r="H10" s="38"/>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A11" s="38"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="43"/>
+      <c r="I10" s="55"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A11" s="55"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="69"/>
       <c r="D11" s="5">
         <v>3</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="38"/>
+      <c r="G11" s="55"/>
       <c r="H11" s="38"/>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A12" s="47"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="44"/>
+      <c r="I11" s="55"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A12" s="67"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="70"/>
       <c r="D12" s="5">
         <v>4</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1">
+      <c r="G12" s="67"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="67"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickBot="1">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -4648,20 +4843,21 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:I1"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="B4:B7"/>
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="G4:G7"/>
-    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="I4:I7"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="B9:B12"/>
     <mergeCell ref="C9:C12"/>
     <mergeCell ref="G9:G12"/>
-    <mergeCell ref="H9:H12"/>
+    <mergeCell ref="I9:I12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4669,10 +4865,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4680,22 +4876,23 @@
     <col min="3" max="3" width="26.28515625" customWidth="1"/>
     <col min="5" max="5" width="29.140625" customWidth="1"/>
     <col min="6" max="6" width="22.28515625" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="7" max="8" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="25.5" customHeight="1" thickBot="1">
-      <c r="A1" s="48" t="s">
+    <row r="1" spans="1:9" ht="25.5" customHeight="1" thickBot="1">
+      <c r="A1" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1">
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -4718,10 +4915,13 @@
         <v>6</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -4743,65 +4943,70 @@
       <c r="G3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="4"/>
+      <c r="I3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A4" s="37" t="s">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A4" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="57" t="s">
         <v>101</v>
       </c>
-      <c r="C4" s="42"/>
+      <c r="C4" s="68"/>
       <c r="D4" s="5">
         <v>1</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="6"/>
-      <c r="G4" s="37" t="s">
+      <c r="G4" s="54" t="s">
         <v>103</v>
       </c>
       <c r="H4" s="37"/>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A5" s="38"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="43"/>
+      <c r="I4" s="54"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A5" s="55"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="69"/>
       <c r="D5" s="5">
         <v>2</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="6"/>
-      <c r="G5" s="38"/>
+      <c r="G5" s="55"/>
       <c r="H5" s="38"/>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A6" s="38"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="43"/>
+      <c r="I5" s="55"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A6" s="55"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="69"/>
       <c r="D6" s="5">
         <v>3</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="38"/>
+      <c r="G6" s="55"/>
       <c r="H6" s="38"/>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A7" s="38"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="43"/>
+      <c r="I6" s="55"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A7" s="55"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="69"/>
       <c r="D7" s="5">
         <v>4</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="6"/>
-      <c r="G7" s="38"/>
+      <c r="G7" s="55"/>
       <c r="H7" s="38"/>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1">
+      <c r="I7" s="55"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -4810,60 +5015,65 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A9" s="37" t="s">
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A9" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="57" t="s">
         <v>102</v>
       </c>
-      <c r="C9" s="42"/>
+      <c r="C9" s="68"/>
       <c r="D9" s="5">
         <v>1</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="6"/>
-      <c r="G9" s="37"/>
+      <c r="G9" s="54"/>
       <c r="H9" s="37"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A10" s="38"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="43"/>
+      <c r="I9" s="54"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A10" s="55"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="69"/>
       <c r="D10" s="5">
         <v>2</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="38"/>
+      <c r="G10" s="55"/>
       <c r="H10" s="38"/>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A11" s="38"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="43"/>
+      <c r="I10" s="55"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A11" s="55"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="69"/>
       <c r="D11" s="5">
         <v>3</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="38"/>
+      <c r="G11" s="55"/>
       <c r="H11" s="38"/>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A12" s="47"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="44"/>
+      <c r="I11" s="55"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A12" s="67"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="70"/>
       <c r="D12" s="5">
         <v>4</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1">
+      <c r="G12" s="67"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="67"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickBot="1">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -4872,20 +5082,21 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:I1"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="B4:B7"/>
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="G4:G7"/>
-    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="I4:I7"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="B9:B12"/>
     <mergeCell ref="C9:C12"/>
     <mergeCell ref="G9:G12"/>
-    <mergeCell ref="H9:H12"/>
+    <mergeCell ref="I9:I12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4893,10 +5104,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4904,22 +5115,23 @@
     <col min="3" max="3" width="26.28515625" customWidth="1"/>
     <col min="5" max="5" width="29.140625" customWidth="1"/>
     <col min="6" max="6" width="22.28515625" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="7" max="8" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="36" customHeight="1" thickBot="1">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:9" ht="36" customHeight="1" thickBot="1">
+      <c r="A1" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -4942,10 +5154,13 @@
         <v>6</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -4967,18 +5182,19 @@
       <c r="G3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="4"/>
+      <c r="I3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="63.75" thickBot="1">
-      <c r="A4" s="37" t="s">
+    <row r="4" spans="1:9" ht="63.75" thickBot="1">
+      <c r="A4" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="57" t="s">
         <v>104</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="68" t="s">
         <v>106</v>
       </c>
       <c r="D4" s="5">
@@ -4990,15 +5206,16 @@
       <c r="F4" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="G4" s="37" t="s">
-        <v>115</v>
+      <c r="G4" s="54" t="s">
+        <v>146</v>
       </c>
       <c r="H4" s="37"/>
-    </row>
-    <row r="5" spans="1:8" ht="32.25" thickBot="1">
-      <c r="A5" s="38"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="43"/>
+      <c r="I4" s="54"/>
+    </row>
+    <row r="5" spans="1:9" ht="32.25" thickBot="1">
+      <c r="A5" s="55"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="69"/>
       <c r="D5" s="5">
         <v>2</v>
       </c>
@@ -5008,13 +5225,14 @@
       <c r="F5" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="G5" s="38"/>
+      <c r="G5" s="55"/>
       <c r="H5" s="38"/>
-    </row>
-    <row r="6" spans="1:8" ht="74.25" thickBot="1">
-      <c r="A6" s="38"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="43"/>
+      <c r="I5" s="55"/>
+    </row>
+    <row r="6" spans="1:9" ht="74.25" thickBot="1">
+      <c r="A6" s="55"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="69"/>
       <c r="D6" s="5">
         <v>3</v>
       </c>
@@ -5024,13 +5242,16 @@
       <c r="F6" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-    </row>
-    <row r="7" spans="1:8" ht="74.25" thickBot="1">
-      <c r="A7" s="38"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="43"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="I6" s="55"/>
+    </row>
+    <row r="7" spans="1:9" ht="74.25" thickBot="1">
+      <c r="A7" s="55"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="69"/>
       <c r="D7" s="5">
         <v>4</v>
       </c>
@@ -5040,10 +5261,11 @@
       <c r="F7" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1">
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1">
       <c r="A8" s="17"/>
       <c r="B8" s="18"/>
       <c r="C8" s="20"/>
@@ -5051,9 +5273,10 @@
       <c r="E8" s="7"/>
       <c r="F8" s="6"/>
       <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1">
+      <c r="H8" s="55"/>
+      <c r="I8" s="17"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1">
       <c r="A9" s="17"/>
       <c r="B9" s="18"/>
       <c r="C9" s="20"/>
@@ -5061,9 +5284,10 @@
       <c r="E9" s="7"/>
       <c r="F9" s="6"/>
       <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1">
+      <c r="H9" s="55"/>
+      <c r="I9" s="17"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -5072,60 +5296,65 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A11" s="37" t="s">
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A11" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="C11" s="42"/>
+      <c r="C11" s="68"/>
       <c r="D11" s="5">
         <v>1</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="37"/>
+      <c r="G11" s="54"/>
       <c r="H11" s="37"/>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A12" s="38"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="43"/>
+      <c r="I11" s="54"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A12" s="55"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="69"/>
       <c r="D12" s="5">
         <v>2</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="38"/>
+      <c r="G12" s="55"/>
       <c r="H12" s="38"/>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A13" s="38"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="43"/>
+      <c r="I12" s="55"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A13" s="55"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="69"/>
       <c r="D13" s="5">
         <v>3</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="6"/>
-      <c r="G13" s="38"/>
+      <c r="G13" s="55"/>
       <c r="H13" s="38"/>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" thickBot="1">
-      <c r="A14" s="47"/>
-      <c r="B14" s="41"/>
-      <c r="C14" s="44"/>
+      <c r="I13" s="55"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A14" s="67"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="70"/>
       <c r="D14" s="5">
         <v>4</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="6"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" thickBot="1">
+      <c r="G14" s="67"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="67"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -5134,20 +5363,22 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A1:H1"/>
+  <mergeCells count="12">
+    <mergeCell ref="A1:I1"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="B4:B7"/>
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="G4:G7"/>
-    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="I4:I7"/>
+    <mergeCell ref="H6:H9"/>
     <mergeCell ref="A11:A14"/>
     <mergeCell ref="B11:B14"/>
     <mergeCell ref="C11:C14"/>
     <mergeCell ref="G11:G14"/>
-    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="I11:I14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>